<commit_message>
Add in more experiment results.
</commit_message>
<xml_diff>
--- a/experiments/meth1-logs/chunk-size/1g.xlsx
+++ b/experiments/meth1-logs/chunk-size/1g.xlsx
@@ -8,14 +8,16 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="211" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="PQ Sort" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Merge Sort" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="50G" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
   <si>
     <t>Read Model</t>
   </si>
@@ -81,16 +83,61 @@
   </si>
   <si>
     <t>70</t>
+  </si>
+  <si>
+    <t>Network Model</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>First-Chunk</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Network-2G</t>
+  </si>
+  <si>
+    <t>Observed</t>
+  </si>
+  <si>
+    <t># 1</t>
+  </si>
+  <si>
+    <t>50GB</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>cmd-read</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="#,###"/>
+    <numFmt numFmtId="169" formatCode="0%"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -172,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -191,6 +238,30 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -265,7 +336,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -326,7 +397,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$5:$B$18</c:f>
+              <c:f>'PQ Sort'!$B$5:$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -376,7 +447,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$18</c:f>
+              <c:f>'PQ Sort'!$D$5:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -460,7 +531,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$5:$B$18</c:f>
+              <c:f>'PQ Sort'!$B$5:$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -510,7 +581,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$18</c:f>
+              <c:f>'PQ Sort'!$E$5:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -574,11 +645,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="29067211"/>
-        <c:axId val="36659842"/>
+        <c:axId val="59344363"/>
+        <c:axId val="85418156"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="29067211"/>
+        <c:axId val="59344363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -614,14 +685,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="36659842"/>
+        <c:crossAx val="85418156"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36659842"/>
+        <c:axId val="85418156"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +737,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="29067211"/>
+        <c:crossAx val="59344363"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -691,7 +762,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -752,7 +823,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$6:$B$12</c:f>
+              <c:f>'PQ Sort'!$B$6:$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -781,7 +852,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$6:$F$12</c:f>
+              <c:f>'PQ Sort'!$F$6:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -824,11 +895,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="4381769"/>
-        <c:axId val="74611404"/>
+        <c:axId val="74887596"/>
+        <c:axId val="30692376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4381769"/>
+        <c:axId val="74887596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,14 +935,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74611404"/>
+        <c:crossAx val="30692376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74611404"/>
+        <c:axId val="30692376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,7 +967,213 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="4381769"/>
+        <c:crossAx val="74887596"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>50G!$C$18,50G!$C$20,50G!$C$22,50G!$C$24,50G!$C$26,50G!$C$28,50G!$C$30,50G!$C$32,50G!$C$34,50G!$C$36,50G!$C$38,50G!$C$40,50G!$C$42,50G!$C$44,50G!$C$46,50G!$C$48,50G!$C$50,50G!$C$52,50G!$C$54,50G!$C$56,50G!$C$58,50G!$C$60,50G!$C$62,50G!$C$64,50G!$C$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>191330</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>168088</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>168779</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>164360</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>162905</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>161475</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>158894</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>161105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>161521</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>154980</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>153510</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149168</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>149930</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>146401</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>146075</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>147882</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>141965</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>139077</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>136192</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>133463</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>130388</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>127841</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>131761</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>128637</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>128750</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars/>
+          <c:downBars/>
+        </c:upDownBars>
+        <c:marker val="0"/>
+        <c:axId val="32757565"/>
+        <c:axId val="40858318"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="32757565"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="40858318"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="40858318"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="32757565"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -986,6 +1263,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>20880</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>90720</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>8280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3511800" y="507240"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -994,7 +1306,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J53" activeCellId="0" sqref="J53"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1313,4 +1625,984 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">B2/B1</f>
+        <v>32.5732899022801</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <f aca="false">(D6-E6)/E6</f>
+        <v>-0.0368098159509203</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>10485</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <f aca="false">(D7-E7)/E7</f>
+        <v>-0.0306748466257669</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">A8*100/1024/1024</f>
+        <v>100</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <f aca="false">(D8-E8)/E8</f>
+        <v>0.398773006134969</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2621440</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <f aca="false">A9*100/1024/1024</f>
+        <v>250</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>49.9</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <f aca="false">(D9-E9)/E9</f>
+        <v>0.530674846625767</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>5242880</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">A10*100/1024/1024</f>
+        <v>500</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <f aca="false">(D10-E10)/E10</f>
+        <v>0.634969325153374</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>7864320</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">A11*100/1024/1024</f>
+        <v>750</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <f aca="false">(D11-E11)/E11</f>
+        <v>0.717791411042945</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>60.1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <f aca="false">(D12-E12)/E12</f>
+        <v>0.843558282208589</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>75.9</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <f aca="false">(D13-E13)/E13</f>
+        <v>1.32822085889571</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D68"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <f aca="false">C5+C7</f>
+        <v>4571.66123778502</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <f aca="false">B3/2000*C6</f>
+        <v>4071.66123778502</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <f aca="false">B3/B1</f>
+        <v>162.866449511401</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">B3/B2</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">2000/B2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <f aca="false">SUM(C11:C12)</f>
+        <v>4425.561</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <f aca="false">(C66+C64+C64+C62+C60+C58+C56+C54+C52+C50+C48+C46+C44+C42+C40+C38+C36+C34+C32+C30+C28+C26+C24+C22+C20+C18)/1000</f>
+        <v>3873.114</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <f aca="false">(C67+C65+C63+C61+C59+C57+C55+C53+C51+C49+C47+C45+C43+C41+C39+C37+C35+C33+C31+C29+C27+C25+C23+C21+C19)/1000</f>
+        <v>552.447</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="8" t="n">
+        <f aca="false">SUM(C70:C71)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="9" t="n">
+        <f aca="false">C10/C4</f>
+        <v>0.968042199501247</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>20971520</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>191330</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="6" t="n">
+        <v>22908</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6" t="n">
+        <v>168088</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="n">
+        <v>21973</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="6" t="n">
+        <v>168779</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6" t="n">
+        <v>22022</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="6" t="n">
+        <v>164360</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="6" t="n">
+        <v>22039</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" s="6" t="n">
+        <v>162905</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="6" t="n">
+        <v>22101</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C28" s="6" t="n">
+        <v>161475</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C29" s="6" t="n">
+        <v>22046</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C30" s="6" t="n">
+        <v>158894</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C31" s="6" t="n">
+        <v>22215</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C32" s="6" t="n">
+        <v>161105</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C33" s="6" t="n">
+        <v>22025</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6" t="n">
+        <v>161521</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C35" s="6" t="n">
+        <v>22162</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C36" s="6" t="n">
+        <v>154980</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C37" s="6" t="n">
+        <v>22067</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6" t="n">
+        <v>153510</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C39" s="6" t="n">
+        <v>22111</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C40" s="6" t="n">
+        <v>149168</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C41" s="6" t="n">
+        <v>21980</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C42" s="6" t="n">
+        <v>149930</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C43" s="6" t="n">
+        <v>22166</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C44" s="6" t="n">
+        <v>146401</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C45" s="6" t="n">
+        <v>22033</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C46" s="6" t="n">
+        <v>146075</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C47" s="6" t="n">
+        <v>22002</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C48" s="6" t="n">
+        <v>147882</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C49" s="6" t="n">
+        <v>22077</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C50" s="6" t="n">
+        <v>141965</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C51" s="6" t="n">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C52" s="6" t="n">
+        <v>139077</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C53" s="6" t="n">
+        <v>22013</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C54" s="6" t="n">
+        <v>136192</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C55" s="6" t="n">
+        <v>22188</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C56" s="6" t="n">
+        <v>133463</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C57" s="6" t="n">
+        <v>21973</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C58" s="6" t="n">
+        <v>130388</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C59" s="6" t="n">
+        <v>22040</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C60" s="6" t="n">
+        <v>127841</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C61" s="6" t="n">
+        <v>22041</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C62" s="6" t="n">
+        <v>131761</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C63" s="6" t="n">
+        <v>22011</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C64" s="6" t="n">
+        <v>128637</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C65" s="6" t="n">
+        <v>22085</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C66" s="6" t="n">
+        <v>128750</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C67" s="6" t="n">
+        <v>22169</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C68" s="6" t="n">
+        <v>4297646</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>